<commit_message>
concluida a parte de cadastro de sessoes, menos no que se refera a episodios. uma consulta geral foi implementada mas seus resultados nao estao sendo apresentados da melhor forma
</commit_message>
<xml_diff>
--- a/Project Tables.xlsx
+++ b/Project Tables.xlsx
@@ -111,9 +111,6 @@
     <t>evaluetion</t>
   </si>
   <si>
-    <t>mode</t>
-  </si>
-  <si>
     <t>comment</t>
   </si>
   <si>
@@ -142,6 +139,9 @@
   </si>
   <si>
     <t>tagCode</t>
+  </si>
+  <si>
+    <t>modeCode</t>
   </si>
 </sst>
 </file>
@@ -685,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -854,7 +854,7 @@
       <c r="B16" s="2"/>
       <c r="C16" s="3"/>
       <c r="D16" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E16" s="20" t="s">
         <v>12</v>
@@ -891,7 +891,7 @@
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>12</v>
@@ -937,7 +937,7 @@
     <row r="24" spans="2:6" ht="15.75" thickBot="1"/>
     <row r="25" spans="2:6" ht="15.75" thickBot="1">
       <c r="B25" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C25" s="26"/>
       <c r="D25" s="26"/>
@@ -963,7 +963,7 @@
       <c r="B27" s="2"/>
       <c r="C27" s="3"/>
       <c r="D27" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>12</v>
@@ -974,7 +974,7 @@
       <c r="B28" s="2"/>
       <c r="C28" s="3"/>
       <c r="D28" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>12</v>
@@ -1063,7 +1063,7 @@
         <v>14</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>12</v>
@@ -1104,7 +1104,7 @@
         <v>29</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>15</v>
@@ -1142,7 +1142,7 @@
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="4" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>12</v>
@@ -1153,17 +1153,17 @@
       <c r="B45" s="6"/>
       <c r="C45" s="7"/>
       <c r="D45" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F45" s="9"/>
     </row>
     <row r="46" spans="2:6" ht="15.75" thickBot="1"/>
     <row r="47" spans="2:6" ht="15.75" thickBot="1">
       <c r="B47" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C47" s="23"/>
       <c r="D47" s="23"/>

</xml_diff>